<commit_message>
adapted backend code for osparc
</commit_message>
<xml_diff>
--- a/assets/INPUT_FOLDER/input.xlsx
+++ b/assets/INPUT_FOLDER/input.xlsx
@@ -5,36 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3dtholdings-my.sharepoint.com/personal/bpatel_calmi2_org/Documents/Bhavesh/SPARC/SODA-other/Codeathon test code/INPUT_FOLDER/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calmi2\Documents\GitHub\KnowMore-b\assets\INPUT_FOLDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_B78D80A37FF76FFC05FC9890E27DBAB6A0DDF063" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2765297A-F101-4286-820E-40118E889BA9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC39A31-F02D-4B53-BA2B-40945D6BF521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="630" windowWidth="23865" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="3300" windowWidth="16920" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>datasetId</t>
   </si>
 </sst>
 </file>
@@ -436,44 +424,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>